<commit_message>
4/25 goal list update
</commit_message>
<xml_diff>
--- a/scripts/DK64 Randomizer Bingo Goals.xlsx
+++ b/scripts/DK64 Randomizer Bingo Goals.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="153">
   <si>
     <t>Id</t>
   </si>
@@ -130,10 +130,10 @@
     <t>Orange Throwing</t>
   </si>
   <si>
-    <t>Diving</t>
-  </si>
-  <si>
-    <t>Vine Swinging</t>
+    <t>Save the Apple Reward</t>
+  </si>
+  <si>
+    <t>Castle Lanky Tower</t>
   </si>
   <si>
     <t>Barrel Throwing</t>
@@ -181,7 +181,7 @@
     <t>Endgame</t>
   </si>
   <si>
-    <t>Disable the Blastomatic</t>
+    <t>1 Company Coin</t>
   </si>
   <si>
     <t>Complete Dk Arcade Round 2</t>
@@ -476,7 +476,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -487,6 +487,11 @@
       <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="&quot;Aptos Narrow&quot;"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -503,7 +508,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -515,6 +520,12 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1179,31 +1190,27 @@
       <c r="A30" s="2">
         <v>29.0</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="2">
-        <v>1.0</v>
+      <c r="C30" s="5">
+        <v>14.0</v>
       </c>
       <c r="D30" s="3"/>
-      <c r="E30" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="E30" s="1"/>
     </row>
     <row r="31">
       <c r="A31" s="2">
         <v>30.0</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="2">
-        <v>1.0</v>
+      <c r="C31" s="5">
+        <v>14.0</v>
       </c>
       <c r="D31" s="3"/>
-      <c r="E31" s="1" t="s">
-        <v>36</v>
-      </c>
+      <c r="E31" s="1"/>
     </row>
     <row r="32">
       <c r="A32" s="2">
@@ -1389,15 +1396,13 @@
       <c r="A44" s="2">
         <v>43.0</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C44" s="2">
-        <v>20.0</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>55</v>
-      </c>
+      <c r="C44" s="5">
+        <v>12.0</v>
+      </c>
+      <c r="D44" s="1"/>
       <c r="E44" s="3"/>
     </row>
     <row r="45">

</xml_diff>

<commit_message>
4/27 goal list update
keys in vanilla locations
</commit_message>
<xml_diff>
--- a/scripts/DK64 Randomizer Bingo Goals.xlsx
+++ b/scripts/DK64 Randomizer Bingo Goals.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="162">
   <si>
     <t>Id</t>
   </si>
@@ -151,7 +151,7 @@
     <t>Key 1</t>
   </si>
   <si>
-    <t>Key</t>
+    <t>Keys</t>
   </si>
   <si>
     <t>Key 2</t>
@@ -250,13 +250,10 @@
     <t>CBs</t>
   </si>
   <si>
-    <t>Defeat a Boss</t>
-  </si>
-  <si>
-    <t>Boss</t>
-  </si>
-  <si>
-    <t>Defeat 2 Bosses</t>
+    <t>Have 2 Keys</t>
+  </si>
+  <si>
+    <t>Have 3 Keys</t>
   </si>
   <si>
     <t>Defeat Mad Jack</t>
@@ -268,7 +265,7 @@
     <t>Defeat Armydillo 2</t>
   </si>
   <si>
-    <t>Defeat All Bosses</t>
+    <t>All Keys</t>
   </si>
   <si>
     <t>Complete Diddy Lower Cabin</t>
@@ -397,7 +394,7 @@
     <t>Complete All 3 Mincecarts</t>
   </si>
   <si>
-    <t>Vin Diesel</t>
+    <t>Kong Family</t>
   </si>
   <si>
     <t>Pound the X</t>
@@ -457,7 +454,7 @@
     <t>20 Blueprints</t>
   </si>
   <si>
-    <t>Collect The End of Helm</t>
+    <t>Disable the Blastomatic</t>
   </si>
   <si>
     <t>Complete All Lighthouse Area Checks</t>
@@ -470,13 +467,43 @@
   </si>
   <si>
     <t>Complete Both Tiny Car Races</t>
+  </si>
+  <si>
+    <t>400 Coloured Bananas in Crystal Caves</t>
+  </si>
+  <si>
+    <t>400 Coloured Bananas in Fungi Forest</t>
+  </si>
+  <si>
+    <t>400 Coloured Bananas in Gloomy Galleon</t>
+  </si>
+  <si>
+    <t>Have 4 Keys</t>
+  </si>
+  <si>
+    <t>Have 5 Keys</t>
+  </si>
+  <si>
+    <t>70 Golden Bananas</t>
+  </si>
+  <si>
+    <t>80 Golden Bananas</t>
+  </si>
+  <si>
+    <t>DK Isles Summit Barrel</t>
+  </si>
+  <si>
+    <t>All Kasplats in Angry Aztec</t>
+  </si>
+  <si>
+    <t>All Kasplats in Crystal Caves</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -493,6 +520,11 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -508,7 +540,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -522,10 +554,13 @@
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -938,8 +973,8 @@
       <c r="B13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="2">
-        <v>1.0</v>
+      <c r="C13" s="4">
+        <v>2.0</v>
       </c>
       <c r="D13" s="3"/>
       <c r="E13" s="1" t="s">
@@ -1013,8 +1048,8 @@
       <c r="B18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C18" s="2">
-        <v>1.0</v>
+      <c r="C18" s="4">
+        <v>2.0</v>
       </c>
       <c r="D18" s="3"/>
       <c r="E18" s="1" t="s">
@@ -1190,10 +1225,10 @@
       <c r="A30" s="2">
         <v>29.0</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="4">
         <v>14.0</v>
       </c>
       <c r="D30" s="3"/>
@@ -1203,10 +1238,10 @@
       <c r="A31" s="2">
         <v>30.0</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="4">
         <v>14.0</v>
       </c>
       <c r="D31" s="3"/>
@@ -1219,8 +1254,8 @@
       <c r="B32" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C32" s="2">
-        <v>1.0</v>
+      <c r="C32" s="4">
+        <v>2.0</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="1" t="s">
@@ -1264,11 +1299,11 @@
       <c r="B35" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C35" s="2">
-        <v>5.0</v>
+      <c r="C35" s="4">
+        <v>9.0</v>
       </c>
       <c r="D35" s="3"/>
-      <c r="E35" s="1" t="s">
+      <c r="E35" s="5" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1279,11 +1314,11 @@
       <c r="B36" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="4">
         <v>9.0</v>
       </c>
       <c r="D36" s="3"/>
-      <c r="E36" s="1" t="s">
+      <c r="E36" s="5" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1298,7 +1333,7 @@
         <v>11.0</v>
       </c>
       <c r="D37" s="3"/>
-      <c r="E37" s="1" t="s">
+      <c r="E37" s="5" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1309,11 +1344,11 @@
       <c r="B38" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C38" s="2">
-        <v>11.0</v>
+      <c r="C38" s="4">
+        <v>9.0</v>
       </c>
       <c r="D38" s="3"/>
-      <c r="E38" s="1" t="s">
+      <c r="E38" s="5" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1324,11 +1359,11 @@
       <c r="B39" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C39" s="2">
-        <v>13.0</v>
+      <c r="C39" s="4">
+        <v>9.0</v>
       </c>
       <c r="D39" s="3"/>
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="5" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1339,11 +1374,11 @@
       <c r="B40" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C40" s="2">
-        <v>15.0</v>
+      <c r="C40" s="4">
+        <v>9.0</v>
       </c>
       <c r="D40" s="3"/>
-      <c r="E40" s="1" t="s">
+      <c r="E40" s="5" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1354,11 +1389,11 @@
       <c r="B41" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C41" s="2">
-        <v>15.0</v>
+      <c r="C41" s="4">
+        <v>9.0</v>
       </c>
       <c r="D41" s="3"/>
-      <c r="E41" s="1" t="s">
+      <c r="E41" s="5" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1369,11 +1404,11 @@
       <c r="B42" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C42" s="2">
-        <v>15.0</v>
+      <c r="C42" s="4">
+        <v>26.0</v>
       </c>
       <c r="D42" s="3"/>
-      <c r="E42" s="1" t="s">
+      <c r="E42" s="5" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1396,10 +1431,10 @@
       <c r="A44" s="2">
         <v>43.0</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C44" s="4">
         <v>12.0</v>
       </c>
       <c r="D44" s="1"/>
@@ -1645,8 +1680,8 @@
       <c r="B62" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C62" s="2">
-        <v>20.0</v>
+      <c r="C62" s="4">
+        <v>16.0</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>78</v>
@@ -1657,14 +1692,14 @@
       <c r="A63" s="2">
         <v>62.0</v>
       </c>
-      <c r="B63" s="1" t="s">
+      <c r="B63" s="5" t="s">
         <v>79</v>
       </c>
       <c r="C63" s="2">
         <v>4.0</v>
       </c>
-      <c r="D63" s="1" t="s">
-        <v>80</v>
+      <c r="D63" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="E63" s="3"/>
     </row>
@@ -1672,14 +1707,14 @@
       <c r="A64" s="2">
         <v>63.0</v>
       </c>
-      <c r="B64" s="1" t="s">
-        <v>81</v>
+      <c r="B64" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="C64" s="2">
         <v>10.0</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>80</v>
+      <c r="D64" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="E64" s="3"/>
     </row>
@@ -1688,14 +1723,14 @@
         <v>64.0</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C65" s="2">
         <v>11.0</v>
       </c>
       <c r="D65" s="3"/>
-      <c r="E65" s="1" t="s">
-        <v>80</v>
+      <c r="E65" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="66">
@@ -1703,14 +1738,14 @@
         <v>65.0</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C66" s="2">
         <v>18.0</v>
       </c>
       <c r="D66" s="3"/>
-      <c r="E66" s="1" t="s">
-        <v>80</v>
+      <c r="E66" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="67">
@@ -1718,28 +1753,28 @@
         <v>66.0</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C67" s="2">
         <v>11.0</v>
       </c>
       <c r="D67" s="3"/>
-      <c r="E67" s="1" t="s">
-        <v>80</v>
+      <c r="E67" s="5" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2">
         <v>67.0</v>
       </c>
-      <c r="B68" s="1" t="s">
-        <v>85</v>
+      <c r="B68" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="C68" s="2">
         <v>25.0</v>
       </c>
-      <c r="D68" s="1" t="s">
-        <v>80</v>
+      <c r="D68" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="E68" s="3"/>
     </row>
@@ -1748,14 +1783,14 @@
         <v>68.0</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C69" s="2">
         <v>8.0</v>
       </c>
       <c r="D69" s="3"/>
       <c r="E69" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="70">
@@ -1763,7 +1798,7 @@
         <v>69.0</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C70" s="2">
         <v>17.0</v>
@@ -1776,7 +1811,7 @@
         <v>70.0</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C71" s="2">
         <v>3.0</v>
@@ -1789,7 +1824,7 @@
         <v>71.0</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C72" s="2">
         <v>5.0</v>
@@ -1802,7 +1837,7 @@
         <v>72.0</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C73" s="2">
         <v>5.0</v>
@@ -1815,7 +1850,7 @@
         <v>73.0</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C74" s="2">
         <v>8.0</v>
@@ -1828,7 +1863,7 @@
         <v>74.0</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C75" s="2">
         <v>5.0</v>
@@ -1841,7 +1876,7 @@
         <v>75.0</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C76" s="2">
         <v>5.0</v>
@@ -1854,7 +1889,7 @@
         <v>76.0</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C77" s="2">
         <v>5.0</v>
@@ -1867,7 +1902,7 @@
         <v>77.0</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C78" s="2">
         <v>2.0</v>
@@ -1880,7 +1915,7 @@
         <v>78.0</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C79" s="2">
         <v>2.0</v>
@@ -1893,7 +1928,7 @@
         <v>79.0</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C80" s="2">
         <v>5.0</v>
@@ -1906,7 +1941,7 @@
         <v>80.0</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C81" s="2">
         <v>6.0</v>
@@ -1919,7 +1954,7 @@
         <v>81.0</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C82" s="2">
         <v>2.0</v>
@@ -1932,7 +1967,7 @@
         <v>82.0</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C83" s="2">
         <v>4.0</v>
@@ -1945,7 +1980,7 @@
         <v>83.0</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C84" s="2">
         <v>3.0</v>
@@ -1958,7 +1993,7 @@
         <v>84.0</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C85" s="2">
         <v>3.0</v>
@@ -1971,7 +2006,7 @@
         <v>85.0</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C86" s="2">
         <v>6.0</v>
@@ -1984,7 +2019,7 @@
         <v>86.0</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C87" s="2">
         <v>3.0</v>
@@ -1997,7 +2032,7 @@
         <v>87.0</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C88" s="2">
         <v>3.0</v>
@@ -2010,7 +2045,7 @@
         <v>88.0</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C89" s="2">
         <v>7.0</v>
@@ -2023,7 +2058,7 @@
         <v>89.0</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C90" s="2">
         <v>4.0</v>
@@ -2036,7 +2071,7 @@
         <v>90.0</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C91" s="2">
         <v>9.0</v>
@@ -2049,7 +2084,7 @@
         <v>91.0</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C92" s="2">
         <v>7.0</v>
@@ -2062,7 +2097,7 @@
         <v>92.0</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C93" s="2">
         <v>7.0</v>
@@ -2075,10 +2110,10 @@
         <v>93.0</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C94" s="2">
-        <v>18.0</v>
+        <v>111</v>
+      </c>
+      <c r="C94" s="4">
+        <v>13.0</v>
       </c>
       <c r="D94" s="3"/>
       <c r="E94" s="3"/>
@@ -2088,7 +2123,7 @@
         <v>94.0</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C95" s="2">
         <v>5.0</v>
@@ -2101,7 +2136,7 @@
         <v>95.0</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C96" s="2">
         <v>14.0</v>
@@ -2114,10 +2149,10 @@
         <v>96.0</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C97" s="2">
-        <v>16.0</v>
+        <v>114</v>
+      </c>
+      <c r="C97" s="4">
+        <v>12.0</v>
       </c>
       <c r="D97" s="3"/>
       <c r="E97" s="3"/>
@@ -2127,7 +2162,7 @@
         <v>97.0</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C98" s="2">
         <v>9.0</v>
@@ -2140,10 +2175,10 @@
         <v>98.0</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C99" s="2">
-        <v>17.0</v>
+        <v>116</v>
+      </c>
+      <c r="C99" s="4">
+        <v>13.0</v>
       </c>
       <c r="D99" s="3"/>
       <c r="E99" s="3"/>
@@ -2153,7 +2188,7 @@
         <v>99.0</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C100" s="2">
         <v>12.0</v>
@@ -2166,7 +2201,7 @@
         <v>100.0</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C101" s="2">
         <v>4.0</v>
@@ -2179,7 +2214,7 @@
         <v>101.0</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C102" s="2">
         <v>14.0</v>
@@ -2192,7 +2227,7 @@
         <v>102.0</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C103" s="2">
         <v>7.0</v>
@@ -2205,7 +2240,7 @@
         <v>103.0</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C104" s="2">
         <v>4.0</v>
@@ -2218,10 +2253,10 @@
         <v>104.0</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C105" s="2">
-        <v>16.0</v>
+        <v>122</v>
+      </c>
+      <c r="C105" s="4">
+        <v>13.0</v>
       </c>
       <c r="D105" s="3"/>
       <c r="E105" s="3"/>
@@ -2231,7 +2266,7 @@
         <v>105.0</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C106" s="2">
         <v>15.0</v>
@@ -2244,7 +2279,7 @@
         <v>106.0</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C107" s="2">
         <v>13.0</v>
@@ -2259,7 +2294,7 @@
         <v>107.0</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C108" s="2">
         <v>10.0</v>
@@ -2274,7 +2309,7 @@
         <v>108.0</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C109" s="2">
         <v>12.0</v>
@@ -2286,8 +2321,8 @@
       <c r="A110" s="2">
         <v>109.0</v>
       </c>
-      <c r="B110" s="1" t="s">
-        <v>128</v>
+      <c r="B110" s="5" t="s">
+        <v>127</v>
       </c>
       <c r="C110" s="2">
         <v>3.0</v>
@@ -2300,7 +2335,7 @@
         <v>110.0</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C111" s="2">
         <v>9.0</v>
@@ -2313,13 +2348,13 @@
         <v>111.0</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C112" s="2">
         <v>19.0</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E112" s="3"/>
     </row>
@@ -2328,13 +2363,13 @@
         <v>112.0</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C113" s="2">
         <v>20.0</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E113" s="3"/>
     </row>
@@ -2343,13 +2378,13 @@
         <v>113.0</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C114" s="2">
         <v>17.0</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E114" s="3"/>
     </row>
@@ -2358,13 +2393,13 @@
         <v>114.0</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C115" s="2">
         <v>17.0</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E115" s="3"/>
     </row>
@@ -2373,13 +2408,13 @@
         <v>115.0</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C116" s="2">
         <v>21.0</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E116" s="3"/>
     </row>
@@ -2388,13 +2423,13 @@
         <v>116.0</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C117" s="2">
         <v>23.0</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E117" s="3"/>
     </row>
@@ -2403,7 +2438,7 @@
         <v>117.0</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C118" s="2">
         <v>14.0</v>
@@ -2416,7 +2451,7 @@
         <v>118.0</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C119" s="2">
         <v>17.0</v>
@@ -2429,7 +2464,7 @@
         <v>119.0</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C120" s="2">
         <v>22.0</v>
@@ -2444,7 +2479,7 @@
         <v>120.0</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C121" s="2">
         <v>15.0</v>
@@ -2457,13 +2492,13 @@
         <v>121.0</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C122" s="2">
         <v>9.0</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E122" s="3"/>
     </row>
@@ -2472,13 +2507,13 @@
         <v>122.0</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C123" s="2">
         <v>18.0</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E123" s="3"/>
     </row>
@@ -2487,13 +2522,13 @@
         <v>123.0</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C124" s="2">
         <v>11.0</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E124" s="3"/>
     </row>
@@ -2502,13 +2537,13 @@
         <v>124.0</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C125" s="2">
         <v>21.0</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E125" s="3"/>
     </row>
@@ -2516,10 +2551,10 @@
       <c r="A126" s="2">
         <v>125.0</v>
       </c>
-      <c r="B126" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="C126" s="2">
+      <c r="B126" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C126" s="4">
         <v>25.0</v>
       </c>
       <c r="D126" s="1" t="s">
@@ -2532,7 +2567,7 @@
         <v>126.0</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C127" s="2">
         <v>24.0</v>
@@ -2545,10 +2580,10 @@
         <v>127.0</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="C128" s="2">
-        <v>24.0</v>
+        <v>149</v>
+      </c>
+      <c r="C128" s="4">
+        <v>19.0</v>
       </c>
       <c r="D128" s="1" t="s">
         <v>78</v>
@@ -2560,7 +2595,7 @@
         <v>128.0</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C129" s="2">
         <v>23.0</v>
@@ -2573,13 +2608,144 @@
         <v>129.0</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C130" s="2">
         <v>11.0</v>
       </c>
       <c r="D130" s="3"/>
       <c r="E130" s="3"/>
+    </row>
+    <row r="131">
+      <c r="A131" s="6">
+        <v>130.0</v>
+      </c>
+      <c r="B131" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C131" s="6">
+        <v>24.0</v>
+      </c>
+      <c r="D131" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="6">
+        <v>131.0</v>
+      </c>
+      <c r="B132" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C132" s="6">
+        <v>22.0</v>
+      </c>
+      <c r="D132" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="6">
+        <v>132.0</v>
+      </c>
+      <c r="B133" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C133" s="6">
+        <v>22.0</v>
+      </c>
+      <c r="D133" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="6">
+        <v>133.0</v>
+      </c>
+      <c r="B134" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="C134" s="6">
+        <v>16.0</v>
+      </c>
+      <c r="D134" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="6">
+        <v>134.0</v>
+      </c>
+      <c r="B135" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C135" s="6">
+        <v>21.0</v>
+      </c>
+      <c r="D135" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="6">
+        <v>135.0</v>
+      </c>
+      <c r="B136" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="C136" s="6">
+        <v>20.0</v>
+      </c>
+      <c r="D136" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="6">
+        <v>136.0</v>
+      </c>
+      <c r="B137" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="C137" s="6">
+        <v>24.0</v>
+      </c>
+      <c r="D137" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="6">
+        <v>137.0</v>
+      </c>
+      <c r="B138" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="C138" s="6">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="6">
+        <v>138.0</v>
+      </c>
+      <c r="B139" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="C139" s="6">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="6">
+        <v>139.0</v>
+      </c>
+      <c r="B140" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="C140" s="6">
+        <v>16.0</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>